<commit_message>
small change to action defaults
</commit_message>
<xml_diff>
--- a/fixed_wf3_template.xlsx
+++ b/fixed_wf3_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ipendleton/Dropbox/Desktop/ESCALATE/ESCALATE_Capture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC2DBCF-FFC8-744A-9063-314D937F94BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3137FC95-028C-3247-8C3D-78C5DA0637CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6340" yWindow="1460" windowWidth="35360" windowHeight="24200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2604,8 +2604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
+      <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -5781,7 +5781,7 @@
         <v>20</v>
       </c>
       <c r="E87" s="116">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="F87" s="78">
         <v>80</v>
@@ -42771,7 +42771,7 @@
       </c>
       <c r="D155" s="78">
         <f>'User Interface'!E87</f>
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="E155" s="78" t="s">
         <v>187</v>

</xml_diff>